<commit_message>
Purchase Payment Test added
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="224">
   <si>
     <t>Hello</t>
   </si>
@@ -185,12 +185,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>Frank</t>
-  </si>
-  <si>
-    <t>Dux</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -206,9 +200,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>testSuccessfulLumpsumPayAddLCPrevMonth</t>
-  </si>
-  <si>
     <t>IL</t>
   </si>
   <si>
@@ -416,9 +407,6 @@
     <t>06</t>
   </si>
   <si>
-    <t>EA21R12</t>
-  </si>
-  <si>
     <t>EF9SIR12</t>
   </si>
   <si>
@@ -428,9 +416,6 @@
     <t>EG6R12</t>
   </si>
   <si>
-    <t>S15RB25DET12</t>
-  </si>
-  <si>
     <t>FC3S13BT12</t>
   </si>
   <si>
@@ -449,30 +434,9 @@
     <t>TE2212</t>
   </si>
   <si>
-    <t>FD3S12</t>
-  </si>
-  <si>
-    <t>S13RB25DET12</t>
-  </si>
-  <si>
     <t>AP1TypeR12</t>
   </si>
   <si>
-    <t>180sxRB25DET12</t>
-  </si>
-  <si>
-    <t>NA6CTypeR12</t>
-  </si>
-  <si>
-    <t>NA1TypeR12</t>
-  </si>
-  <si>
-    <t>TE3312</t>
-  </si>
-  <si>
-    <t>KP111112</t>
-  </si>
-  <si>
     <t>ssN</t>
   </si>
   <si>
@@ -693,15 +657,78 @@
   </si>
   <si>
     <t>1960</t>
+  </si>
+  <si>
+    <t>FC3STD06G20</t>
+  </si>
+  <si>
+    <t>AE864AGTE</t>
+  </si>
+  <si>
+    <t>EA21RRR</t>
+  </si>
+  <si>
+    <t>EF9B16A</t>
+  </si>
+  <si>
+    <t>S14RB26</t>
+  </si>
+  <si>
+    <t>EG6B18C</t>
+  </si>
+  <si>
+    <t>S15RB26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE111 </t>
+  </si>
+  <si>
+    <t>TE222</t>
+  </si>
+  <si>
+    <t>TE333</t>
+  </si>
+  <si>
+    <t>TE444</t>
+  </si>
+  <si>
+    <t>ANG1234</t>
+  </si>
+  <si>
+    <t>TE555</t>
+  </si>
+  <si>
+    <t>NA1TypeRR</t>
+  </si>
+  <si>
+    <t>NA6CTypeRR</t>
+  </si>
+  <si>
+    <t>180SXTYPEX</t>
+  </si>
+  <si>
+    <t>S13RB26</t>
+  </si>
+  <si>
+    <t>FD3STD06G20</t>
+  </si>
+  <si>
+    <t>AP1TypeRR</t>
+  </si>
+  <si>
+    <t>Duke</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>testSuccessfulPurchaseLumpsumPayAdd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -790,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -825,13 +852,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -858,9 +879,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1166,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L111"/>
+  <dimension ref="A1:L124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109:A111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,13 +1224,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>126</v>
+        <v>202</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1220,13 +1238,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>127</v>
+        <v>203</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,13 +1252,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>121</v>
+        <v>204</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1248,13 +1266,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>122</v>
+        <v>205</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1262,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>123</v>
+        <v>206</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>221</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1276,13 +1294,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,13 +1308,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>125</v>
+        <v>208</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,13 +1322,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>128</v>
+        <v>209</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1318,13 +1336,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>129</v>
+        <v>210</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1332,13 +1350,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>130</v>
+        <v>211</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,19 +1364,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1380,13 +1398,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>134</v>
+        <v>220</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1394,13 +1412,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1408,7 +1426,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>133</v>
+        <v>218</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>31</v>
@@ -1422,13 +1440,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>135</v>
+        <v>217</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1436,13 +1454,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>136</v>
+        <v>216</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1450,13 +1468,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>137</v>
+        <v>215</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1464,13 +1482,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>138</v>
+        <v>214</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1478,23 +1496,23 @@
         <v>5</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>139</v>
+        <v>213</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
-      <c r="B24" s="21"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="21"/>
+      <c r="B25" s="19"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1536,34 +1554,34 @@
         <v>17</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>134</v>
+        <v>220</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="H28" s="19">
+      <c r="G28" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="18">
         <v>26</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>37</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1571,34 +1589,34 @@
         <v>17</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>127</v>
+        <v>203</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>162</v>
+        <v>49</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>150</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="31">
+      <c r="G29" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29" s="29">
         <v>25</v>
       </c>
       <c r="I29" s="15" t="s">
         <v>37</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1606,7 +1624,7 @@
         <v>17</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>19</v>
@@ -1621,19 +1639,19 @@
         <v>22</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="K30" s="25" t="s">
-        <v>79</v>
+        <v>106</v>
+      </c>
+      <c r="J30" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K30" s="23" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1641,22 +1659,22 @@
         <v>17</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>53</v>
+        <v>211</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F31" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H31" s="15" t="s">
         <v>34</v>
@@ -1665,10 +1683,10 @@
         <v>38</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1676,34 +1694,34 @@
         <v>17</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>125</v>
+        <v>208</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -1711,34 +1729,34 @@
         <v>17</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" s="27" t="s">
-        <v>119</v>
+        <v>216</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>116</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="H33" s="28" t="s">
-        <v>120</v>
+      <c r="G33" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>117</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>37</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1746,7 +1764,7 @@
         <v>17</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>122</v>
+        <v>205</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>28</v>
@@ -1761,7 +1779,7 @@
         <v>16</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H34" s="15" t="s">
         <v>33</v>
@@ -1770,10 +1788,10 @@
         <v>36</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -1781,7 +1799,7 @@
         <v>17</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>139</v>
+        <v>213</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>18</v>
@@ -1799,16 +1817,16 @@
         <v>10</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K35" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -1816,7 +1834,7 @@
         <v>17</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>19</v>
@@ -1831,7 +1849,7 @@
         <v>16</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H36" s="15" t="s">
         <v>41</v>
@@ -1840,10 +1858,10 @@
         <v>37</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -1851,7 +1869,7 @@
         <v>17</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>123</v>
+        <v>206</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>18</v>
@@ -1866,7 +1884,7 @@
         <v>15</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H37" s="15">
         <v>11</v>
@@ -1875,10 +1893,10 @@
         <v>37</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>45</v>
+        <v>221</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>44</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -1886,7 +1904,7 @@
         <v>17</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>137</v>
+        <v>215</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>19</v>
@@ -1910,10 +1928,10 @@
         <v>37</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -1921,7 +1939,7 @@
         <v>17</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>138</v>
+        <v>214</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>23</v>
@@ -1935,33 +1953,33 @@
       <c r="F39" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="26">
+      <c r="G39" s="24">
         <v>11</v>
       </c>
-      <c r="H39" s="19">
+      <c r="H39" s="18">
         <v>19</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="J39" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K39" s="24" t="s">
-        <v>101</v>
+      <c r="J39" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="K39" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="22"/>
-      <c r="D41" s="23"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="22"/>
-      <c r="D42" s="23"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>2</v>
@@ -1979,30 +1997,30 @@
         <v>4</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>19</v>
@@ -2010,26 +2028,26 @@
       <c r="D44" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="F44" s="25" t="s">
-        <v>79</v>
+      <c r="E44" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="J44" s="15" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L44" s="15" t="s">
         <v>37</v>
@@ -2037,48 +2055,48 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C45" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>118</v>
+        <v>216</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J45" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="K45" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="J45" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K45" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="L45" s="25" t="s">
-        <v>108</v>
+      <c r="L45" s="23" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>137</v>
+        <v>215</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>19</v>
@@ -2087,36 +2105,36 @@
         <v>25</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="J46" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="K46" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="L46" s="25" t="s">
-        <v>212</v>
+        <v>138</v>
+      </c>
+      <c r="J46" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="K46" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="L46" s="23" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>138</v>
+        <v>214</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>23</v>
@@ -2125,36 +2143,36 @@
         <v>24</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J47" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="K47" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="L47" s="25" t="s">
-        <v>213</v>
+        <v>142</v>
+      </c>
+      <c r="J47" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="K47" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="L47" s="23" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>139</v>
+        <v>213</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>18</v>
@@ -2163,396 +2181,408 @@
         <v>20</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="H48" s="25" t="s">
-        <v>209</v>
+        <v>196</v>
+      </c>
+      <c r="H48" s="23" t="s">
+        <v>197</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="J48" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="K48" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="J48" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="K48" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="L48" s="25" t="s">
-        <v>186</v>
+      <c r="L48" s="23" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G49" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="H49" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="J49" s="15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="J50" s="15" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="K50" s="15" t="s">
         <v>33</v>
       </c>
       <c r="L50" s="15" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B51" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G51" s="3" t="s">
+      <c r="H51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="J51" s="15" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="K51" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L51" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="L51" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F54" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F55" s="20">
-        <v>10000</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F56" s="20">
-        <v>12000</v>
+        <v>172</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>132</v>
+        <v>165</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" s="20">
-        <v>500</v>
+        <v>141</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>33</v>
+        <v>204</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F58" s="20">
-        <v>5</v>
+        <v>111</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C59" s="18">
-        <v>14</v>
+        <v>205</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E59" s="18">
-        <v>2016</v>
-      </c>
-      <c r="F59" s="20">
-        <v>300000</v>
+        <v>90</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C60" s="18">
-        <v>24</v>
+        <v>206</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E60" s="18">
-        <v>2017</v>
-      </c>
-      <c r="F60" s="20">
-        <v>500000</v>
+        <v>108</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D63" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>50</v>
+      <c r="A63" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>125</v>
+        <v>165</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>34</v>
+        <v>175</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>177</v>
-      </c>
+      <c r="A65" s="2"/>
       <c r="B65" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>151</v>
+        <v>33</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>153</v>
+        <v>42</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>132</v>
+      <c r="A66" s="2"/>
+      <c r="B66" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>114</v>
+        <v>175</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F66" s="15" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>133</v>
+      <c r="A67" s="2"/>
+      <c r="B67" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>135</v>
+      <c r="A68" s="2"/>
+      <c r="B68" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>111</v>
+        <v>175</v>
       </c>
       <c r="E68" s="15" t="s">
         <v>37</v>
@@ -2562,608 +2592,576 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>136</v>
+      <c r="A69" s="2"/>
+      <c r="B69" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="D69" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F70" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E69" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F69" s="15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="15" t="s">
+      <c r="C71" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="F71" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E70" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F70" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C71" s="15" t="s">
+      <c r="E72" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F72" s="15" t="s">
         <v>188</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E71" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F71" s="15" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D72" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="F72" s="15" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
-      <c r="B73" s="3" t="s">
-        <v>126</v>
+      <c r="B73" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>33</v>
+        <v>175</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F73" s="15" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>187</v>
+        <v>90</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F74" s="15" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>43</v>
+        <v>178</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>40</v>
+        <v>174</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="F76" s="15" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
-      <c r="B77" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D77" s="15" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D79" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E79" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D80" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E77" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="F77" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C78" s="15" t="s">
+      <c r="E80" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F80" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E81" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F81" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C82" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D78" s="15" t="s">
+      <c r="D82" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E83" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F83" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C84" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E78" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F78" s="15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D79" s="15" t="s">
+      <c r="D84" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F84" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B102" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C102" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E102" s="27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B103" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C103" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D103" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E103" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="E79" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="F79" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E80" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F80" s="15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D81" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="E81" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F81" s="15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="B82" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D82" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E82" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F82" s="15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
-      <c r="B83" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D83" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E83" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="F83" s="15" t="s">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B104" s="11" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
-      <c r="B84" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C84" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D84" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="E84" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="F84" s="15" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="C104" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D104" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E104" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D105" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C106" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D106" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C107" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D107" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D108" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D109" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D110" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D112" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B113" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B88" s="1" t="s">
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="16"/>
+      <c r="B115" s="19"/>
+      <c r="C115" s="16"/>
+      <c r="D115" s="16"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I116" s="28"/>
+      <c r="J116" s="28"/>
+      <c r="K116" s="28"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B118" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C89" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D89" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E89" s="29" t="s">
+      <c r="C118" s="31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C119" s="30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B120" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C122" s="30" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B124" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C90" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D90" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="E90" s="29" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C91" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D91" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E91" s="29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D92" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B93" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D93" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D94" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B95" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C95" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D95" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B96" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C96" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D96" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B97" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D97" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D98" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B99" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C99" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D99" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B100" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C100" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D100" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="16"/>
-      <c r="B102" s="21"/>
-      <c r="C102" s="16"/>
-      <c r="D102" s="16"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I103" s="30"/>
-      <c r="J103" s="30"/>
-      <c r="K103" s="30"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B105" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C105" s="34" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B106" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="C106" s="32" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B108" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B109" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="C109" s="32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B110" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>